<commit_message>
Alterações na arquitetura, conforme orientações após Sprint 2
</commit_message>
<xml_diff>
--- a/documentacao/P&I/Sprint 2 - Todos os entregáveis/Planilha de Gestão de Riscos.xlsx
+++ b/documentacao/P&I/Sprint 2 - Todos os entregáveis/Planilha de Gestão de Riscos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\Repositorios\sdpiar\documentacao\P&amp;I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\Repositorios\sdpiar\documentacao\P&amp;I\Sprint 2 - Todos os entregáveis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F63CEF64-DC68-4201-A7E3-7DE8060EEA51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ABB59C-92B5-4F6F-B480-E7B8A0821596}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF82710C-C4CB-4DEB-A4E4-4868FE420171}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Alto(3)</t>
   </si>
   <si>
-    <t>Nosso grupo tem a quantidade mínima de pessoas, uma a menos faria diferença</t>
-  </si>
-  <si>
     <t>Não fazer as atividades designadas</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>1 dia</t>
+  </si>
+  <si>
+    <t>Todos os outros integrantes do grupo são muito bons e podem suprir a falta de um elemento.</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A62A1B8-29AB-48F1-A3C3-532BE985E7DC}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,10 +619,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -643,13 +643,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -657,25 +657,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -695,10 +695,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -707,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -719,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>